<commit_message>
Added boiling point correlation capability
</commit_message>
<xml_diff>
--- a/data/Solver_Input/gani_prop_table.xlsx
+++ b/data/Solver_Input/gani_prop_table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="7900" yWindow="5640" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>CH3 (1)</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>tb</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -453,6 +456,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -538,7 +548,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -550,6 +560,7 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -885,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DQ30"/>
+  <dimension ref="A1:DQ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DH1" workbookViewId="0">
-      <selection activeCell="DR11" sqref="DR11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5657,6 +5668,371 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14" spans="1:121">
+      <c r="A14" s="7">
+        <v>0.88939999999999997</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.60329999999999995</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.2878</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1.7827</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1.8432999999999999</v>
+      </c>
+      <c r="G14" s="7">
+        <v>1.7117</v>
+      </c>
+      <c r="H14" s="7">
+        <v>1.7957000000000001</v>
+      </c>
+      <c r="I14" s="7">
+        <v>1.8880999999999999</v>
+      </c>
+      <c r="J14" s="7">
+        <v>3.1242999999999999</v>
+      </c>
+      <c r="K14" s="7">
+        <v>0.92969999999999997</v>
+      </c>
+      <c r="L14" s="7">
+        <v>1.6254</v>
+      </c>
+      <c r="M14" s="7">
+        <v>1.9669000000000001</v>
+      </c>
+      <c r="N14" s="7">
+        <v>1.9478</v>
+      </c>
+      <c r="O14" s="7">
+        <v>1.7444</v>
+      </c>
+      <c r="P14" s="7">
+        <v>3.2151999999999998</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>4.4013999999999998</v>
+      </c>
+      <c r="R14" s="7">
+        <v>3.5668000000000002</v>
+      </c>
+      <c r="S14" s="7">
+        <v>3.8967000000000001</v>
+      </c>
+      <c r="T14" s="7">
+        <v>2.8525999999999998</v>
+      </c>
+      <c r="U14" s="7">
+        <v>3.6360000000000001</v>
+      </c>
+      <c r="V14" s="7">
+        <v>3.3953000000000002</v>
+      </c>
+      <c r="W14" s="7">
+        <v>3.1459000000000001</v>
+      </c>
+      <c r="X14" s="7">
+        <v>2.2536</v>
+      </c>
+      <c r="Y14" s="7">
+        <v>1.6249</v>
+      </c>
+      <c r="Z14" s="7">
+        <v>1.1556999999999999</v>
+      </c>
+      <c r="AA14" s="7">
+        <v>2.5891999999999999</v>
+      </c>
+      <c r="AB14" s="7">
+        <v>3.1656</v>
+      </c>
+      <c r="AC14" s="7">
+        <v>2.5983000000000001</v>
+      </c>
+      <c r="AD14" s="7">
+        <v>3.1375999999999999</v>
+      </c>
+      <c r="AE14" s="7">
+        <v>2.6126999999999998</v>
+      </c>
+      <c r="AF14" s="7">
+        <v>1.5780000000000001</v>
+      </c>
+      <c r="AG14" s="7">
+        <v>2.1646999999999998</v>
+      </c>
+      <c r="AH14" s="7">
+        <v>1.2171000000000001</v>
+      </c>
+      <c r="AI14" s="7">
+        <v>5.4736000000000002</v>
+      </c>
+      <c r="AJ14" s="7">
+        <v>6.28</v>
+      </c>
+      <c r="AK14" s="7">
+        <v>5.9234</v>
+      </c>
+      <c r="AL14" s="7">
+        <v>5.0525000000000002</v>
+      </c>
+      <c r="AM14" s="7">
+        <v>5.8337000000000003</v>
+      </c>
+      <c r="AN14" s="7">
+        <v>2.9636999999999998</v>
+      </c>
+      <c r="AO14" s="7">
+        <v>2.6947999999999999</v>
+      </c>
+      <c r="AP14" s="7">
+        <v>2.2073</v>
+      </c>
+      <c r="AQ14" s="7">
+        <v>3.93</v>
+      </c>
+      <c r="AR14" s="7">
+        <v>3.56</v>
+      </c>
+      <c r="AS14" s="7">
+        <v>4.5796999999999999</v>
+      </c>
+      <c r="AT14" s="7">
+        <v>2.6293000000000002</v>
+      </c>
+      <c r="AU14" s="7">
+        <v>5.7618999999999998</v>
+      </c>
+      <c r="AV14" s="7">
+        <v>5.0766999999999998</v>
+      </c>
+      <c r="AW14" s="7">
+        <v>6.0837000000000003</v>
+      </c>
+      <c r="AX14" s="7">
+        <v>3.2913999999999999</v>
+      </c>
+      <c r="AY14" s="7">
+        <v>3.665</v>
+      </c>
+      <c r="AZ14" s="7">
+        <v>2.6495000000000002</v>
+      </c>
+      <c r="BA14" s="7">
+        <v>2.3677999999999999</v>
+      </c>
+      <c r="BB14" s="7">
+        <v>2.5644999999999998</v>
+      </c>
+      <c r="BC14" s="7">
+        <v>1.7824</v>
+      </c>
+      <c r="BD14" s="7">
+        <v>0.94420000000000004</v>
+      </c>
+      <c r="BE14" s="7">
+        <v>7.2644000000000002</v>
+      </c>
+      <c r="BF14" s="7">
+        <v>1.288</v>
+      </c>
+      <c r="BG14" s="7">
+        <v>0.61150000000000004</v>
+      </c>
+      <c r="BH14" s="7">
+        <v>1.1738999999999999</v>
+      </c>
+      <c r="BI14" s="7">
+        <v>2.6446000000000001</v>
+      </c>
+      <c r="BJ14" s="7">
+        <v>2.8881000000000001</v>
+      </c>
+      <c r="BK14" s="7">
+        <v>2.3086000000000002</v>
+      </c>
+      <c r="BL14" s="7">
+        <v>1.9162999999999999</v>
+      </c>
+      <c r="BM14" s="7">
+        <v>1.0081</v>
+      </c>
+      <c r="BN14" s="7">
+        <v>10.3428</v>
+      </c>
+      <c r="BO14" s="7">
+        <v>0</v>
+      </c>
+      <c r="BP14" s="7">
+        <v>0</v>
+      </c>
+      <c r="BQ14" s="7">
+        <v>7.6904000000000003</v>
+      </c>
+      <c r="BR14" s="7">
+        <v>0</v>
+      </c>
+      <c r="BS14" s="7">
+        <v>6.7821999999999996</v>
+      </c>
+      <c r="BT14" s="7">
+        <v>5.5566000000000004</v>
+      </c>
+      <c r="BU14" s="7">
+        <v>5.4248000000000003</v>
+      </c>
+      <c r="BV14" s="7">
+        <v>3.6796000000000002</v>
+      </c>
+      <c r="BW14" s="7">
+        <v>3.6762999999999999</v>
+      </c>
+      <c r="BX14" s="7">
+        <v>2.6812</v>
+      </c>
+      <c r="BY14" s="7">
+        <v>5.7092999999999998</v>
+      </c>
+      <c r="BZ14" s="7">
+        <v>5.8259999999999996</v>
+      </c>
+      <c r="CA14" s="7">
+        <v>-0.1157</v>
+      </c>
+      <c r="CB14" s="7">
+        <v>-4.8899999999999999E-2</v>
+      </c>
+      <c r="CC14" s="7">
+        <v>0.17979999999999999</v>
+      </c>
+      <c r="CD14" s="7">
+        <v>0.31890000000000002</v>
+      </c>
+      <c r="CE14" s="7">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="CF14" s="7">
+        <v>0.47449999999999998</v>
+      </c>
+      <c r="CG14" s="7">
+        <v>0.35630000000000001</v>
+      </c>
+      <c r="CH14" s="7">
+        <v>0.19189999999999999</v>
+      </c>
+      <c r="CI14" s="7">
+        <v>0.19570000000000001</v>
+      </c>
+      <c r="CJ14" s="7">
+        <v>0.34889999999999999</v>
+      </c>
+      <c r="CK14" s="7">
+        <v>0.15890000000000001</v>
+      </c>
+      <c r="CL14" s="7">
+        <v>6.6799999999999998E-2</v>
+      </c>
+      <c r="CM14" s="7">
+        <v>-0.1406</v>
+      </c>
+      <c r="CN14" s="7">
+        <v>-0.09</v>
+      </c>
+      <c r="CO14" s="7">
+        <v>5.11E-2</v>
+      </c>
+      <c r="CP14" s="7">
+        <v>0.68840000000000001</v>
+      </c>
+      <c r="CQ14" s="7">
+        <v>-0.1074</v>
+      </c>
+      <c r="CR14" s="7">
+        <v>2.24E-2</v>
+      </c>
+      <c r="CS14" s="7">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="CT14" s="7">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="CU14" s="7">
+        <v>7.3499999999999996E-2</v>
+      </c>
+      <c r="CV14" s="7">
+        <v>-0.1552</v>
+      </c>
+      <c r="CW14" s="7">
+        <v>0.78010000000000002</v>
+      </c>
+      <c r="CX14" s="7">
+        <v>-0.23830000000000001</v>
+      </c>
+      <c r="CY14" s="7">
+        <v>0.4456</v>
+      </c>
+      <c r="CZ14" s="7">
+        <v>-0.19769999999999999</v>
+      </c>
+      <c r="DA14" s="7">
+        <v>8.3500000000000005E-2</v>
+      </c>
+      <c r="DB14" s="7">
+        <v>-0.53849999999999998</v>
+      </c>
+      <c r="DC14" s="7">
+        <v>-0.6331</v>
+      </c>
+      <c r="DD14" s="7">
+        <v>1.4108000000000001</v>
+      </c>
+      <c r="DE14" s="7">
+        <v>-6.9000000000000006E-2</v>
+      </c>
+      <c r="DF14" s="7">
+        <v>1.0682</v>
+      </c>
+      <c r="DG14" s="7">
+        <v>0.42470000000000002</v>
+      </c>
+      <c r="DH14" s="7">
+        <v>0.24990000000000001</v>
+      </c>
+      <c r="DI14" s="7">
+        <v>0.1134</v>
+      </c>
+      <c r="DJ14" s="7">
+        <v>-0.2596</v>
+      </c>
+      <c r="DK14" s="7">
+        <v>0.44080000000000003</v>
+      </c>
+      <c r="DL14" s="7">
+        <v>-0.1168</v>
+      </c>
+      <c r="DM14" s="7">
+        <v>-0.3201</v>
+      </c>
+      <c r="DN14" s="7">
+        <v>-0.44529999999999997</v>
+      </c>
+      <c r="DO14" s="7">
+        <v>-0.67759999999999998</v>
+      </c>
+      <c r="DP14" s="7">
+        <v>-0.36780000000000002</v>
+      </c>
+      <c r="DQ14" s="7">
+        <v>0</v>
+      </c>
+    </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>101</v>
@@ -5715,6 +6091,11 @@
     <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Titanium and TTIP
</commit_message>
<xml_diff>
--- a/data/Solver_Input/gani_prop_table.xlsx
+++ b/data/Solver_Input/gani_prop_table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7900" yWindow="5640" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="2840" yWindow="0" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t>CH3 (1)</t>
   </si>
@@ -421,6 +421,9 @@
   </si>
   <si>
     <t>tb</t>
+  </si>
+  <si>
+    <t>Ti(IV)</t>
   </si>
 </sst>
 </file>
@@ -436,6 +439,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -896,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DQ31"/>
+  <dimension ref="A1:DR31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="DM1" workbookViewId="0">
+      <selection activeCell="DR12" sqref="DR12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -923,7 +927,7 @@
     <col min="121" max="121" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:121">
+    <row r="1" spans="1:122">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1287,8 +1291,11 @@
       <c r="DQ1" t="s">
         <v>129</v>
       </c>
+      <c r="DR1" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="2" spans="1:121">
+    <row r="2" spans="1:122">
       <c r="A2">
         <v>1.6780999999999999</v>
       </c>
@@ -1652,8 +1659,11 @@
       <c r="DQ2">
         <v>0</v>
       </c>
+      <c r="DR2">
+        <v>-2.3504999999999998</v>
+      </c>
     </row>
-    <row r="3" spans="1:121">
+    <row r="3" spans="1:122">
       <c r="A3">
         <v>1.9900000000000001E-2</v>
       </c>
@@ -2017,8 +2027,11 @@
       <c r="DQ3">
         <v>0</v>
       </c>
+      <c r="DR3">
+        <v>2.555E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:121">
+    <row r="4" spans="1:122">
       <c r="A4">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -2382,8 +2395,11 @@
       <c r="DQ4">
         <v>0</v>
       </c>
+      <c r="DR4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:121">
+    <row r="5" spans="1:122">
       <c r="A5">
         <v>0.29599999999999999</v>
       </c>
@@ -2747,8 +2763,11 @@
       <c r="DQ5">
         <v>0</v>
       </c>
+      <c r="DR5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:121">
+    <row r="6" spans="1:122">
       <c r="A6">
         <v>4.1159999999999997</v>
       </c>
@@ -3112,8 +3131,11 @@
       <c r="DQ6">
         <v>0</v>
       </c>
+      <c r="DR6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:121">
+    <row r="7" spans="1:122">
       <c r="A7">
         <v>2.6100000000000002E-2</v>
       </c>
@@ -3477,8 +3499,11 @@
       <c r="DQ7">
         <v>0</v>
       </c>
+      <c r="DR7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:121">
+    <row r="8" spans="1:122">
       <c r="A8">
         <v>35.115200000000002</v>
       </c>
@@ -3842,8 +3867,11 @@
       <c r="DQ8">
         <v>0</v>
       </c>
+      <c r="DR8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:121">
+    <row r="9" spans="1:122">
       <c r="A9">
         <v>39.592300000000002</v>
       </c>
@@ -4207,8 +4235,11 @@
       <c r="DQ9">
         <v>0</v>
       </c>
+      <c r="DR9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:121">
+    <row r="10" spans="1:122">
       <c r="A10">
         <v>-9.9231999999999996</v>
       </c>
@@ -4572,8 +4603,11 @@
       <c r="DQ10">
         <v>-5.8400000000000001E-2</v>
       </c>
+      <c r="DR10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:121">
+    <row r="11" spans="1:122">
       <c r="A11">
         <v>15</v>
       </c>
@@ -4937,8 +4971,11 @@
       <c r="DQ11">
         <v>0</v>
       </c>
+      <c r="DR11">
+        <v>47.8</v>
+      </c>
     </row>
-    <row r="12" spans="1:121">
+    <row r="12" spans="1:122">
       <c r="A12" s="1">
         <v>0.90110000000000001</v>
       </c>
@@ -5302,8 +5339,11 @@
       <c r="DQ12">
         <v>0</v>
       </c>
+      <c r="DR12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:121">
+    <row r="13" spans="1:122">
       <c r="A13" s="5">
         <v>0.84799999999999998</v>
       </c>
@@ -5667,8 +5707,11 @@
       <c r="DQ13">
         <v>0</v>
       </c>
+      <c r="DR13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:121">
+    <row r="14" spans="1:122">
       <c r="A14" s="7">
         <v>0.88939999999999997</v>
       </c>
@@ -6030,6 +6073,9 @@
         <v>-0.36780000000000002</v>
       </c>
       <c r="DQ14" s="7">
+        <v>0</v>
+      </c>
+      <c r="DR14">
         <v>0</v>
       </c>
     </row>

</xml_diff>